<commit_message>
update explant work flow
</commit_message>
<xml_diff>
--- a/Explant Work Flow.xlsx
+++ b/Explant Work Flow.xlsx
@@ -286,8 +286,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -349,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -365,6 +367,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -380,6 +383,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,8 +1049,8 @@
       <c r="G12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>11</v>
+      <c r="H12" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8">

</xml_diff>

<commit_message>
update explants and work flow
</commit_message>
<xml_diff>
--- a/Explant Work Flow.xlsx
+++ b/Explant Work Flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="986"/>
+    <workbookView xWindow="17060" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Name (Explant #)</t>
   </si>
@@ -154,12 +154,6 @@
   </si>
   <si>
     <t>running (partial)</t>
-  </si>
-  <si>
-    <t>queueing</t>
-  </si>
-  <si>
-    <t>queueing (partial)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +279,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -342,6 +336,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
@@ -373,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -402,6 +410,16 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,6 +448,10 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1005,8 +1027,11 @@
         <f t="shared" si="0"/>
         <v>0.25926523800000001</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>45</v>
+      <c r="G8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1030,8 +1055,8 @@
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>11</v>
+      <c r="H9" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1055,8 +1080,8 @@
       <c r="G10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>11</v>
+      <c r="H10" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1123,8 +1148,8 @@
       <c r="G13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>44</v>
+      <c r="H13" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1148,8 +1173,8 @@
       <c r="G14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>11</v>
+      <c r="H14" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1174,7 +1199,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1199,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1223,8 +1248,8 @@
       <c r="G17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>11</v>
+      <c r="H17" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1288,8 +1313,11 @@
         <f t="shared" si="0"/>
         <v>1.48820668</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>11</v>
+      <c r="G20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1314,7 +1342,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1381,8 +1409,8 @@
       <c r="G24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>11</v>
+      <c r="H24" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:8">

</xml_diff>

<commit_message>
update remote programs and plots
</commit_message>
<xml_diff>
--- a/Explant Work Flow.xlsx
+++ b/Explant Work Flow.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t>Name (Explant #)</t>
   </si>
@@ -150,20 +150,92 @@
     <t>blue: for comparison plots</t>
   </si>
   <si>
-    <t>running/queued</t>
-  </si>
-  <si>
     <t>8000 more samples - first run</t>
   </si>
   <si>
     <t>second run</t>
+  </si>
+  <si>
+    <t>third run</t>
+  </si>
+  <si>
+    <t>fourth run</t>
+  </si>
+  <si>
+    <t>fifth run</t>
+  </si>
+  <si>
+    <t>DONE! (1)</t>
+  </si>
+  <si>
+    <t>DONE! (2)</t>
+  </si>
+  <si>
+    <t>sixth run</t>
+  </si>
+  <si>
+    <t>DONE! (3)</t>
+  </si>
+  <si>
+    <t>DONE! (4)</t>
+  </si>
+  <si>
+    <t>DONE! (5)</t>
+  </si>
+  <si>
+    <t>DONE! (6)</t>
+  </si>
+  <si>
+    <t>DONE! (7)</t>
+  </si>
+  <si>
+    <t>DONE! (8)</t>
+  </si>
+  <si>
+    <t>DONE! (9)</t>
+  </si>
+  <si>
+    <t>DONE! (10)</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>DONE! (11)</t>
+  </si>
+  <si>
+    <t>DONE! (12)</t>
+  </si>
+  <si>
+    <t>DONE! (13)</t>
+  </si>
+  <si>
+    <t>DONE! (14)</t>
+  </si>
+  <si>
+    <t>seventh run</t>
+  </si>
+  <si>
+    <t>eighth run</t>
+  </si>
+  <si>
+    <t>DONE!</t>
+  </si>
+  <si>
+    <t>1556 (split up)</t>
+  </si>
+  <si>
+    <t>2942 (split up)</t>
+  </si>
+  <si>
+    <t>1411 (split up)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -245,6 +317,11 @@
       <color theme="5" tint="0.39997558519241921"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF8000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -305,7 +382,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -361,8 +438,192 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -395,8 +656,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -424,6 +688,98 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -451,6 +807,98 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -848,7 +1296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -857,7 +1305,7 @@
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="72.75" customHeight="1">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="72.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,13 +1328,31 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -905,7 +1371,7 @@
         <v>0.12690470000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1</v>
       </c>
@@ -941,11 +1407,26 @@
       <c r="M3" s="20">
         <v>1021</v>
       </c>
-      <c r="N3" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="N3" s="23">
+        <v>949</v>
+      </c>
+      <c r="O3" s="17">
+        <v>1171</v>
+      </c>
+      <c r="P3" s="25">
+        <v>1305</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>434</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -963,7 +1444,7 @@
         <v>0.163158574</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>2</v>
       </c>
@@ -996,11 +1477,26 @@
       <c r="L5" s="19">
         <v>981</v>
       </c>
-      <c r="M5" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="M5" s="20">
+        <v>1208</v>
+      </c>
+      <c r="N5" s="23">
+        <v>978</v>
+      </c>
+      <c r="O5" s="17">
+        <v>1127</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="R5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1033,11 +1529,26 @@
       <c r="L6" s="19">
         <v>4</v>
       </c>
-      <c r="M6" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="M6" s="20">
+        <v>1043</v>
+      </c>
+      <c r="N6" s="23">
+        <v>1008</v>
+      </c>
+      <c r="O6" s="17">
+        <v>1065</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="R6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1070,11 +1581,23 @@
       <c r="L7" s="19">
         <v>1384</v>
       </c>
-      <c r="M7" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="M7" s="20">
+        <v>1376</v>
+      </c>
+      <c r="N7" s="23">
+        <v>1413</v>
+      </c>
+      <c r="O7" s="17">
+        <v>931</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1107,11 +1630,23 @@
       <c r="L8" s="19">
         <v>1203</v>
       </c>
-      <c r="M8" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="M8" s="20">
+        <v>1497</v>
+      </c>
+      <c r="N8" s="23">
+        <v>1352</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1141,11 +1676,26 @@
       <c r="K9" s="18">
         <v>4</v>
       </c>
-      <c r="L9" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="L9" s="19">
+        <v>1944</v>
+      </c>
+      <c r="M9" s="20">
+        <v>1739</v>
+      </c>
+      <c r="N9" s="23">
+        <v>1959</v>
+      </c>
+      <c r="O9" s="17">
+        <v>634</v>
+      </c>
+      <c r="P9" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1178,11 +1728,23 @@
       <c r="L10" s="19">
         <v>1435</v>
       </c>
-      <c r="M10" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="M10" s="22">
+        <v>1478</v>
+      </c>
+      <c r="N10" s="23">
+        <v>1512</v>
+      </c>
+      <c r="O10" s="17">
+        <v>825</v>
+      </c>
+      <c r="P10" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1762,7 @@
         <v>0.44211647700000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1230,11 +1792,26 @@
       <c r="K12" s="18">
         <v>3</v>
       </c>
-      <c r="L12" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="L12" s="19">
+        <v>1991</v>
+      </c>
+      <c r="M12" s="22">
+        <v>1738</v>
+      </c>
+      <c r="N12" s="23">
+        <v>1712</v>
+      </c>
+      <c r="O12" s="17">
+        <v>930</v>
+      </c>
+      <c r="P12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1264,11 +1841,17 @@
       <c r="K13" s="18">
         <v>2638</v>
       </c>
-      <c r="L13" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="L13" s="19">
+        <v>2884</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1298,11 +1881,20 @@
       <c r="K14" s="18">
         <v>2411</v>
       </c>
-      <c r="L14" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="L14" s="19">
+        <v>2801</v>
+      </c>
+      <c r="M14" s="22">
+        <v>180</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1332,11 +1924,20 @@
       <c r="K15" s="18">
         <v>2044</v>
       </c>
-      <c r="L15" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="L15" s="19">
+        <v>1963</v>
+      </c>
+      <c r="M15" s="22">
+        <v>1993</v>
+      </c>
+      <c r="N15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1369,11 +1970,17 @@
       <c r="L16" s="19">
         <v>2093</v>
       </c>
-      <c r="M16" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="M16" s="22">
+        <v>1576</v>
+      </c>
+      <c r="N16" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1406,11 +2013,17 @@
       <c r="L17" s="19">
         <v>2276</v>
       </c>
-      <c r="M17" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="M17" s="22">
+        <v>957</v>
+      </c>
+      <c r="N17" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1437,11 +2050,29 @@
       <c r="J18" s="17">
         <v>1786</v>
       </c>
-      <c r="K18" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="K18" s="18">
+        <v>384</v>
+      </c>
+      <c r="L18" s="21">
+        <v>1742</v>
+      </c>
+      <c r="M18" s="20">
+        <v>1971</v>
+      </c>
+      <c r="N18" s="23">
+        <v>1693</v>
+      </c>
+      <c r="O18" s="17">
+        <v>424</v>
+      </c>
+      <c r="P18" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1459,7 +2090,7 @@
         <v>1.26231285</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>15</v>
       </c>
@@ -1489,11 +2120,20 @@
       <c r="K20" s="18">
         <v>1990</v>
       </c>
-      <c r="L20" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="L20" s="19">
+        <v>1972</v>
+      </c>
+      <c r="M20" s="22">
+        <v>1959</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1520,11 +2160,23 @@
       <c r="J21" s="17">
         <v>3268</v>
       </c>
-      <c r="K21" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="K21" s="18">
+        <v>478</v>
+      </c>
+      <c r="L21" s="21">
+        <v>3390</v>
+      </c>
+      <c r="M21" s="22">
+        <v>864</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="O21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1551,11 +2203,20 @@
       <c r="J22" s="17">
         <v>2323</v>
       </c>
-      <c r="K22" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="K22" s="18">
+        <v>3113</v>
+      </c>
+      <c r="L22" s="21">
+        <v>2564</v>
+      </c>
+      <c r="M22" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -1573,7 +2234,7 @@
         <v>2.23192149</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>18</v>
       </c>
@@ -1603,11 +2264,20 @@
       <c r="K24" s="18">
         <v>1637</v>
       </c>
-      <c r="L24" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="L24" s="21">
+        <v>2618</v>
+      </c>
+      <c r="M24" s="22">
+        <v>1407</v>
+      </c>
+      <c r="N24" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="O24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -1616,21 +2286,21 @@
       </c>
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:17">
       <c r="A30" s="14"/>
       <c r="B30" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="12"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:17">
       <c r="A31" s="14"/>
       <c r="B31" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:17">
       <c r="A32" s="14"/>
       <c r="B32" s="16" t="s">
         <v>40</v>

</xml_diff>